<commit_message>
different ttest fixes uneven sample size
new plots too
</commit_message>
<xml_diff>
--- a/Results/Pooled Analyses/SfN2017/SfN2017Stat.xlsx
+++ b/Results/Pooled Analyses/SfN2017/SfN2017Stat.xlsx
@@ -417,13 +417,13 @@
         <v>42.906607601363916</v>
       </c>
       <c r="G1">
-        <v>0.11240476970696628</v>
+        <v>0.12816055735067355</v>
       </c>
       <c r="H1">
-        <v>0.12634470500210804</v>
+        <v>0.18375715967599693</v>
       </c>
       <c r="I1">
-        <v>4.965486765097181E-2</v>
+        <v>0.12492995561981513</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -446,13 +446,13 @@
         <v>81.243616792486719</v>
       </c>
       <c r="G2">
-        <v>8.0229237812893969E-2</v>
+        <v>9.0655737310379486E-2</v>
       </c>
       <c r="H2">
-        <v>0.67424330752237138</v>
+        <v>0.62510601173592995</v>
       </c>
       <c r="I2">
-        <v>0.43670933092298059</v>
+        <v>0.41973996405031877</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -475,13 +475,13 @@
         <v>1.4632486671878027</v>
       </c>
       <c r="G3">
-        <v>0.8148049779602905</v>
+        <v>0.81367253694917996</v>
       </c>
       <c r="H3">
-        <v>0.69535441451958202</v>
+        <v>0.72448108008498235</v>
       </c>
       <c r="I3">
-        <v>0.72237026357261303</v>
+        <v>0.63899740950181672</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -504,13 +504,13 @@
         <v>33.722511120900883</v>
       </c>
       <c r="G4">
-        <v>8.8937693240543278E-3</v>
+        <v>9.7880777824103111E-3</v>
       </c>
       <c r="H4">
-        <v>8.9964324268324694E-2</v>
+        <v>3.186017212454903E-2</v>
       </c>
       <c r="I4">
-        <v>0.53690883106579934</v>
+        <v>0.31874223744050778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more results, more plots, more problems
</commit_message>
<xml_diff>
--- a/Results/Pooled Analyses/SfN2017/SfN2017Stat.xlsx
+++ b/Results/Pooled Analyses/SfN2017/SfN2017Stat.xlsx
@@ -399,118 +399,118 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>-55.791136972183757</v>
+        <v>-53.392709111029731</v>
       </c>
       <c r="B1">
-        <v>-61.365095862296542</v>
+        <v>-55.6188407187203</v>
       </c>
       <c r="C1">
-        <v>-27.531378652604456</v>
+        <v>-27.9252905327618</v>
       </c>
       <c r="D1">
-        <v>-37.762883695405819</v>
+        <v>-38.044571325913239</v>
       </c>
       <c r="E1">
-        <v>53.711929198622897</v>
+        <v>49.853236446571145</v>
       </c>
       <c r="F1">
-        <v>32.143682366416748</v>
+        <v>24.865290349462029</v>
       </c>
       <c r="G1">
-        <v>0.40960741944514489</v>
+        <v>0.71611381944429187</v>
       </c>
       <c r="H1">
-        <v>9.0472346061661768E-2</v>
+        <v>7.6556153168828411E-2</v>
       </c>
       <c r="I1">
-        <v>2.7436341956109341E-2</v>
+        <v>1.7908940363758365E-2</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-38.265657782277543</v>
+        <v>-35.301389668524692</v>
       </c>
       <c r="B2">
-        <v>-24.291650076975756</v>
+        <v>-21.096290110667503</v>
       </c>
       <c r="C2">
-        <v>5.1706703126243765</v>
+        <v>4.3509948160231708</v>
       </c>
       <c r="D2">
-        <v>1.3939126098884329</v>
+        <v>1.13678158720719</v>
       </c>
       <c r="E2">
-        <v>120.84412572533708</v>
+        <v>102.09694055269313</v>
       </c>
       <c r="F2">
-        <v>132.30456670550939</v>
+        <v>841.61971847202858</v>
       </c>
       <c r="G2">
-        <v>5.5909900238340311E-2</v>
+        <v>4.9292072964076998E-2</v>
       </c>
       <c r="H2">
-        <v>0.61281071818259569</v>
+        <v>0.66716632437757439</v>
       </c>
       <c r="I2">
-        <v>0.89129400957000948</v>
+        <v>0.36027259808856049</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>-30.663001844359705</v>
+        <v>-26.385158702470903</v>
       </c>
       <c r="B3">
-        <v>-30.499553181412921</v>
+        <v>-24.939424988609087</v>
       </c>
       <c r="C3">
-        <v>-0.11363045430050019</v>
+        <v>-1.4989208996281305</v>
       </c>
       <c r="D3">
-        <v>-2.2241167957266343</v>
+        <v>2.0893944206969048</v>
       </c>
       <c r="E3">
-        <v>62.610577147951744</v>
+        <v>16.767145981410874</v>
       </c>
       <c r="F3">
-        <v>31.655898445891278</v>
+        <v>85.741375495763535</v>
       </c>
       <c r="G3">
-        <v>0.98770901047789372</v>
+        <v>0.88959344251944805</v>
       </c>
       <c r="H3">
-        <v>0.88476948706406833</v>
+        <v>0.7952215365661579</v>
       </c>
       <c r="I3">
-        <v>0.54400946795608029</v>
+        <v>0.30395104643883963</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>-137.14675433539168</v>
+        <v>-128.26333134283314</v>
       </c>
       <c r="B4">
-        <v>-100.21465985352671</v>
+        <v>-96.030651582788735</v>
       </c>
       <c r="C4">
-        <v>-109.1843641996068</v>
+        <v>-104.44950967422911</v>
       </c>
       <c r="D4">
-        <v>-71.305598883634374</v>
+        <v>-71.222603796937065</v>
       </c>
       <c r="E4">
-        <v>18.090064833617088</v>
+        <v>18.462148713722247</v>
       </c>
       <c r="F4">
-        <v>31.198239573148481</v>
+        <v>28.151443458276059</v>
       </c>
       <c r="G4">
-        <v>1.1006120814778739E-2</v>
+        <v>1.9075380041754363E-2</v>
       </c>
       <c r="H4">
-        <v>1.8372078681928E-2</v>
+        <v>2.8513848259217267E-2</v>
       </c>
       <c r="I4">
-        <v>0.21787321669005977</v>
+        <v>0.31846951538707147</v>
       </c>
     </row>
   </sheetData>
@@ -585,27 +585,27 @@
       </c>
       <c r="B5" s="2">
         <f>INDEX(Sheet1!A1:I4,1,1)</f>
-        <v>-55.791136972183757</v>
+        <v>-53.392709111029731</v>
       </c>
       <c r="C5" s="2">
         <f>INDEX(Sheet1!B1:J4,1,1)</f>
-        <v>-61.365095862296542</v>
+        <v>-55.6188407187203</v>
       </c>
       <c r="D5" s="2">
         <f>INDEX(Sheet1!C1:K4,1,1)</f>
-        <v>-27.531378652604456</v>
+        <v>-27.9252905327618</v>
       </c>
       <c r="E5" s="2">
         <f>INDEX(Sheet1!D1:L4,1,1)</f>
-        <v>-37.762883695405819</v>
+        <v>-38.044571325913239</v>
       </c>
       <c r="F5" s="3">
         <f>INDEX(Sheet1!E1:M4,1,1)</f>
-        <v>53.711929198622897</v>
+        <v>49.853236446571145</v>
       </c>
       <c r="G5" s="3">
         <f>INDEX(Sheet1!F1:N4,1,1)</f>
-        <v>32.143682366416748</v>
+        <v>24.865290349462029</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -614,27 +614,27 @@
       </c>
       <c r="B6" s="2">
         <f>INDEX(Sheet1!A2:I5,1,1)</f>
-        <v>-38.265657782277543</v>
+        <v>-35.301389668524692</v>
       </c>
       <c r="C6" s="2">
         <f>INDEX(Sheet1!B2:J5,1,1)</f>
-        <v>-24.291650076975756</v>
+        <v>-21.096290110667503</v>
       </c>
       <c r="D6" s="2">
         <f>INDEX(Sheet1!C2:K5,1,1)</f>
-        <v>5.1706703126243765</v>
+        <v>4.3509948160231708</v>
       </c>
       <c r="E6" s="2">
         <f>INDEX(Sheet1!D2:L5,1,1)</f>
-        <v>1.3939126098884329</v>
+        <v>1.13678158720719</v>
       </c>
       <c r="F6" s="3">
         <f>INDEX(Sheet1!E2:M5,1,1)</f>
-        <v>120.84412572533708</v>
+        <v>102.09694055269313</v>
       </c>
       <c r="G6" s="3">
         <f>INDEX(Sheet1!F2:N5,1,1)</f>
-        <v>132.30456670550939</v>
+        <v>841.61971847202858</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -643,27 +643,27 @@
       </c>
       <c r="B7" s="2">
         <f>INDEX(Sheet1!A3:I6,1,1)</f>
-        <v>-30.663001844359705</v>
+        <v>-26.385158702470903</v>
       </c>
       <c r="C7" s="2">
         <f>INDEX(Sheet1!B3:J6,1,1)</f>
-        <v>-30.499553181412921</v>
+        <v>-24.939424988609087</v>
       </c>
       <c r="D7" s="2">
         <f>INDEX(Sheet1!C3:K6,1,1)</f>
-        <v>-0.11363045430050019</v>
+        <v>-1.4989208996281305</v>
       </c>
       <c r="E7" s="2">
         <f>INDEX(Sheet1!D3:L6,1,1)</f>
-        <v>-2.2241167957266343</v>
+        <v>2.0893944206969048</v>
       </c>
       <c r="F7" s="3">
         <f>INDEX(Sheet1!E3:M6,1,1)</f>
-        <v>62.610577147951744</v>
+        <v>16.767145981410874</v>
       </c>
       <c r="G7" s="3">
         <f>INDEX(Sheet1!F3:N6,1,1)</f>
-        <v>31.655898445891278</v>
+        <v>85.741375495763535</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -672,27 +672,27 @@
       </c>
       <c r="B8" s="2">
         <f>INDEX(Sheet1!A4:I7,1,1)</f>
-        <v>-137.14675433539168</v>
+        <v>-128.26333134283314</v>
       </c>
       <c r="C8" s="2">
         <f>INDEX(Sheet1!B4:J7,1,1)</f>
-        <v>-100.21465985352671</v>
+        <v>-96.030651582788735</v>
       </c>
       <c r="D8" s="2">
         <f>INDEX(Sheet1!C4:K7,1,1)</f>
-        <v>-109.1843641996068</v>
+        <v>-104.44950967422911</v>
       </c>
       <c r="E8" s="2">
         <f>INDEX(Sheet1!D4:L7,1,1)</f>
-        <v>-71.305598883634374</v>
+        <v>-71.222603796937065</v>
       </c>
       <c r="F8" s="3">
         <f>INDEX(Sheet1!E4:M7,1,1)</f>
-        <v>18.090064833617088</v>
+        <v>18.462148713722247</v>
       </c>
       <c r="G8" s="3">
         <f>INDEX(Sheet1!F4:N7,1,1)</f>
-        <v>31.198239573148481</v>
+        <v>28.151443458276059</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results. some values re fixed
Need to fix the values. they dont match
</commit_message>
<xml_diff>
--- a/Results/Pooled Analyses/SfN2017/SfN2017Stat.xlsx
+++ b/Results/Pooled Analyses/SfN2017/SfN2017Stat.xlsx
@@ -399,118 +399,118 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>-53.392709111029731</v>
+        <v>-60.452222850300473</v>
       </c>
       <c r="B1">
-        <v>-55.6188407187203</v>
+        <v>-46.815454639102917</v>
       </c>
       <c r="C1">
-        <v>-27.9252905327618</v>
+        <v>32.234359752781799</v>
       </c>
       <c r="D1">
-        <v>-38.044571325913239</v>
+        <v>17.574269392807071</v>
       </c>
       <c r="E1">
-        <v>49.853236446571145</v>
+        <v>54.662865537799988</v>
       </c>
       <c r="F1">
-        <v>24.865290349462029</v>
+        <v>23.739806067855504</v>
       </c>
       <c r="G1">
-        <v>0.71611381944429187</v>
+        <v>8.0253940776943547E-2</v>
       </c>
       <c r="H1">
-        <v>7.6556153168828411E-2</v>
+        <v>3.9251599338186678E-2</v>
       </c>
       <c r="I1">
-        <v>1.7908940363758365E-2</v>
+        <v>0.1792914238915696</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-35.301389668524692</v>
+        <v>-38.568789654826901</v>
       </c>
       <c r="B2">
-        <v>-21.096290110667503</v>
+        <v>-37.058758765709939</v>
       </c>
       <c r="C2">
-        <v>4.3509948160231708</v>
+        <v>39.652384484547859</v>
       </c>
       <c r="D2">
-        <v>1.13678158720719</v>
+        <v>22.233071697874685</v>
       </c>
       <c r="E2">
-        <v>102.09694055269313</v>
+        <v>112.06024561874294</v>
       </c>
       <c r="F2">
-        <v>841.61971847202858</v>
+        <v>44.848392915193649</v>
       </c>
       <c r="G2">
-        <v>4.9292072964076998E-2</v>
+        <v>0.77604792271659129</v>
       </c>
       <c r="H2">
-        <v>0.66716632437757439</v>
+        <v>2.338784622668174E-2</v>
       </c>
       <c r="I2">
-        <v>0.36027259808856049</v>
+        <v>2.6059326658168607E-2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>-26.385158702470903</v>
+        <v>-32.855435271891913</v>
       </c>
       <c r="B3">
-        <v>-24.939424988609087</v>
+        <v>-18.719792706390411</v>
       </c>
       <c r="C3">
-        <v>-1.4989208996281305</v>
+        <v>24.886237802842782</v>
       </c>
       <c r="D3">
-        <v>2.0893944206969048</v>
+        <v>27.028819409305996</v>
       </c>
       <c r="E3">
-        <v>16.767145981410874</v>
+        <v>73.584706403222611</v>
       </c>
       <c r="F3">
-        <v>85.741375495763535</v>
+        <v>98.551787665001754</v>
       </c>
       <c r="G3">
-        <v>0.88959344251944805</v>
+        <v>1.5320075979370769E-2</v>
       </c>
       <c r="H3">
-        <v>0.7952215365661579</v>
+        <v>0.8090047428123075</v>
       </c>
       <c r="I3">
-        <v>0.30395104643883963</v>
+        <v>0.51605489471206889</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>-128.26333134283314</v>
+        <v>-97.92097308662197</v>
       </c>
       <c r="B4">
-        <v>-96.030651582788735</v>
+        <v>-74.541131221758448</v>
       </c>
       <c r="C4">
-        <v>-104.44950967422911</v>
+        <v>23.813821668604032</v>
       </c>
       <c r="D4">
-        <v>-71.222603796937065</v>
+        <v>24.80804778585167</v>
       </c>
       <c r="E4">
-        <v>18.462148713722247</v>
+        <v>23.508923601223366</v>
       </c>
       <c r="F4">
-        <v>28.151443458276059</v>
+        <v>33.700803808855369</v>
       </c>
       <c r="G4">
-        <v>1.9075380041754363E-2</v>
+        <v>1.990728685446809E-2</v>
       </c>
       <c r="H4">
-        <v>2.8513848259217267E-2</v>
+        <v>0.9249022513445011</v>
       </c>
       <c r="I4">
-        <v>0.31846951538707147</v>
+        <v>0.56478935286805643</v>
       </c>
     </row>
   </sheetData>
@@ -585,27 +585,27 @@
       </c>
       <c r="B5" s="2">
         <f>INDEX(Sheet1!A1:I4,1,1)</f>
-        <v>-53.392709111029731</v>
+        <v>-60.452222850300473</v>
       </c>
       <c r="C5" s="2">
         <f>INDEX(Sheet1!B1:J4,1,1)</f>
-        <v>-55.6188407187203</v>
+        <v>-46.815454639102917</v>
       </c>
       <c r="D5" s="2">
         <f>INDEX(Sheet1!C1:K4,1,1)</f>
-        <v>-27.9252905327618</v>
+        <v>32.234359752781799</v>
       </c>
       <c r="E5" s="2">
         <f>INDEX(Sheet1!D1:L4,1,1)</f>
-        <v>-38.044571325913239</v>
+        <v>17.574269392807071</v>
       </c>
       <c r="F5" s="3">
         <f>INDEX(Sheet1!E1:M4,1,1)</f>
-        <v>49.853236446571145</v>
+        <v>54.662865537799988</v>
       </c>
       <c r="G5" s="3">
         <f>INDEX(Sheet1!F1:N4,1,1)</f>
-        <v>24.865290349462029</v>
+        <v>23.739806067855504</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -614,27 +614,27 @@
       </c>
       <c r="B6" s="2">
         <f>INDEX(Sheet1!A2:I5,1,1)</f>
-        <v>-35.301389668524692</v>
+        <v>-38.568789654826901</v>
       </c>
       <c r="C6" s="2">
         <f>INDEX(Sheet1!B2:J5,1,1)</f>
-        <v>-21.096290110667503</v>
+        <v>-37.058758765709939</v>
       </c>
       <c r="D6" s="2">
         <f>INDEX(Sheet1!C2:K5,1,1)</f>
-        <v>4.3509948160231708</v>
+        <v>39.652384484547859</v>
       </c>
       <c r="E6" s="2">
         <f>INDEX(Sheet1!D2:L5,1,1)</f>
-        <v>1.13678158720719</v>
+        <v>22.233071697874685</v>
       </c>
       <c r="F6" s="3">
         <f>INDEX(Sheet1!E2:M5,1,1)</f>
-        <v>102.09694055269313</v>
+        <v>112.06024561874294</v>
       </c>
       <c r="G6" s="3">
         <f>INDEX(Sheet1!F2:N5,1,1)</f>
-        <v>841.61971847202858</v>
+        <v>44.848392915193649</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -643,27 +643,27 @@
       </c>
       <c r="B7" s="2">
         <f>INDEX(Sheet1!A3:I6,1,1)</f>
-        <v>-26.385158702470903</v>
+        <v>-32.855435271891913</v>
       </c>
       <c r="C7" s="2">
         <f>INDEX(Sheet1!B3:J6,1,1)</f>
-        <v>-24.939424988609087</v>
+        <v>-18.719792706390411</v>
       </c>
       <c r="D7" s="2">
         <f>INDEX(Sheet1!C3:K6,1,1)</f>
-        <v>-1.4989208996281305</v>
+        <v>24.886237802842782</v>
       </c>
       <c r="E7" s="2">
         <f>INDEX(Sheet1!D3:L6,1,1)</f>
-        <v>2.0893944206969048</v>
+        <v>27.028819409305996</v>
       </c>
       <c r="F7" s="3">
         <f>INDEX(Sheet1!E3:M6,1,1)</f>
-        <v>16.767145981410874</v>
+        <v>73.584706403222611</v>
       </c>
       <c r="G7" s="3">
         <f>INDEX(Sheet1!F3:N6,1,1)</f>
-        <v>85.741375495763535</v>
+        <v>98.551787665001754</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -672,27 +672,27 @@
       </c>
       <c r="B8" s="2">
         <f>INDEX(Sheet1!A4:I7,1,1)</f>
-        <v>-128.26333134283314</v>
+        <v>-97.92097308662197</v>
       </c>
       <c r="C8" s="2">
         <f>INDEX(Sheet1!B4:J7,1,1)</f>
-        <v>-96.030651582788735</v>
+        <v>-74.541131221758448</v>
       </c>
       <c r="D8" s="2">
         <f>INDEX(Sheet1!C4:K7,1,1)</f>
-        <v>-104.44950967422911</v>
+        <v>23.813821668604032</v>
       </c>
       <c r="E8" s="2">
         <f>INDEX(Sheet1!D4:L7,1,1)</f>
-        <v>-71.222603796937065</v>
+        <v>24.80804778585167</v>
       </c>
       <c r="F8" s="3">
         <f>INDEX(Sheet1!E4:M7,1,1)</f>
-        <v>18.462148713722247</v>
+        <v>23.508923601223366</v>
       </c>
       <c r="G8" s="3">
         <f>INDEX(Sheet1!F4:N7,1,1)</f>
-        <v>28.151443458276059</v>
+        <v>33.700803808855369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerunning the pooled analyses
New results based off of some recent changes. After I switch to the new method of pooling. These values should not change.
</commit_message>
<xml_diff>
--- a/Results/Pooled Analyses/SfN2017/SfN2017Stat.xlsx
+++ b/Results/Pooled Analyses/SfN2017/SfN2017Stat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djsmith\Documents\MATLAB\Dissociating-Role-of-Feedback-in-Voice-Motor-Control\Results\Pooled Analyses\SfN2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\MATLAB\Dissociating-Role-of-Feedback-in-Voice-Motor-Control\Results\Pooled Analyses\SfN2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -460,28 +460,28 @@
         <v>-32.855435271891913</v>
       </c>
       <c r="B3">
-        <v>-18.719792706390411</v>
+        <v>-19.364946692964853</v>
       </c>
       <c r="C3">
         <v>24.886237802842782</v>
       </c>
       <c r="D3">
-        <v>27.028819409305996</v>
+        <v>26.523555712032437</v>
       </c>
       <c r="E3">
         <v>73.584706403222611</v>
       </c>
       <c r="F3">
-        <v>98.551787665001754</v>
+        <v>96.300037659891615</v>
       </c>
       <c r="G3">
-        <v>1.5320075979370769E-2</v>
+        <v>1.7952714771327243E-2</v>
       </c>
       <c r="H3">
-        <v>0.8090047428123075</v>
+        <v>0.84980120462270137</v>
       </c>
       <c r="I3">
-        <v>0.51605489471206889</v>
+        <v>0.54459077402851874</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -489,28 +489,28 @@
         <v>-97.92097308662197</v>
       </c>
       <c r="B4">
-        <v>-74.541131221758448</v>
+        <v>-78.496639998254906</v>
       </c>
       <c r="C4">
         <v>23.813821668604032</v>
       </c>
       <c r="D4">
-        <v>24.80804778585167</v>
+        <v>24.106221427066124</v>
       </c>
       <c r="E4">
         <v>23.508923601223366</v>
       </c>
       <c r="F4">
-        <v>33.700803808855369</v>
+        <v>32.330468954191872</v>
       </c>
       <c r="G4">
-        <v>1.990728685446809E-2</v>
+        <v>6.403038201997592E-2</v>
       </c>
       <c r="H4">
-        <v>0.9249022513445011</v>
+        <v>0.97731086153151481</v>
       </c>
       <c r="I4">
-        <v>0.56478935286805643</v>
+        <v>0.60931132471887395</v>
       </c>
     </row>
   </sheetData>
@@ -647,7 +647,7 @@
       </c>
       <c r="C7" s="2">
         <f>INDEX(Sheet1!B3:J6,1,1)</f>
-        <v>-18.719792706390411</v>
+        <v>-19.364946692964853</v>
       </c>
       <c r="D7" s="2">
         <f>INDEX(Sheet1!C3:K6,1,1)</f>
@@ -655,7 +655,7 @@
       </c>
       <c r="E7" s="2">
         <f>INDEX(Sheet1!D3:L6,1,1)</f>
-        <v>27.028819409305996</v>
+        <v>26.523555712032437</v>
       </c>
       <c r="F7" s="3">
         <f>INDEX(Sheet1!E3:M6,1,1)</f>
@@ -663,7 +663,7 @@
       </c>
       <c r="G7" s="3">
         <f>INDEX(Sheet1!F3:N6,1,1)</f>
-        <v>98.551787665001754</v>
+        <v>96.300037659891615</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -676,7 +676,7 @@
       </c>
       <c r="C8" s="2">
         <f>INDEX(Sheet1!B4:J7,1,1)</f>
-        <v>-74.541131221758448</v>
+        <v>-78.496639998254906</v>
       </c>
       <c r="D8" s="2">
         <f>INDEX(Sheet1!C4:K7,1,1)</f>
@@ -684,7 +684,7 @@
       </c>
       <c r="E8" s="2">
         <f>INDEX(Sheet1!D4:L7,1,1)</f>
-        <v>24.80804778585167</v>
+        <v>24.106221427066124</v>
       </c>
       <c r="F8" s="3">
         <f>INDEX(Sheet1!E4:M7,1,1)</f>
@@ -692,7 +692,7 @@
       </c>
       <c r="G8" s="3">
         <f>INDEX(Sheet1!F4:N7,1,1)</f>
-        <v>33.700803808855369</v>
+        <v>32.330468954191872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I had removed a run of trials
For whatever reason I had decided to throw away a whole run of trials that I deemed not good enough. I no longer need to go through such steps. Now I dont any catch for a specific run to throw away. Updated the results file, and the plots
</commit_message>
<xml_diff>
--- a/Results/Pooled Analyses/SfN2017/SfN2017Stat.xlsx
+++ b/Results/Pooled Analyses/SfN2017/SfN2017Stat.xlsx
@@ -399,31 +399,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>-60.452222850300473</v>
+        <v>-48.242649518285319</v>
       </c>
       <c r="B1">
         <v>-46.815454639102917</v>
       </c>
       <c r="C1">
-        <v>32.234359752781799</v>
+        <v>25.467418578267914</v>
       </c>
       <c r="D1">
         <v>17.574269392807071</v>
       </c>
       <c r="E1">
-        <v>54.662865537799988</v>
+        <v>56.051484437544296</v>
       </c>
       <c r="F1">
         <v>23.739806067855504</v>
       </c>
       <c r="G1">
-        <v>8.0253940776943547E-2</v>
+        <v>0.82077446204103555</v>
       </c>
       <c r="H1">
-        <v>3.9251599338186678E-2</v>
+        <v>0.15002041082696027</v>
       </c>
       <c r="I1">
-        <v>0.1792914238915696</v>
+        <v>6.2873566091793481E-2</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -585,7 +585,7 @@
       </c>
       <c r="B5" s="2">
         <f>INDEX(Sheet1!A1:I4,1,1)</f>
-        <v>-60.452222850300473</v>
+        <v>-48.242649518285319</v>
       </c>
       <c r="C5" s="2">
         <f>INDEX(Sheet1!B1:J4,1,1)</f>
@@ -593,7 +593,7 @@
       </c>
       <c r="D5" s="2">
         <f>INDEX(Sheet1!C1:K4,1,1)</f>
-        <v>32.234359752781799</v>
+        <v>25.467418578267914</v>
       </c>
       <c r="E5" s="2">
         <f>INDEX(Sheet1!D1:L4,1,1)</f>
@@ -601,7 +601,7 @@
       </c>
       <c r="F5" s="3">
         <f>INDEX(Sheet1!E1:M4,1,1)</f>
-        <v>54.662865537799988</v>
+        <v>56.051484437544296</v>
       </c>
       <c r="G5" s="3">
         <f>INDEX(Sheet1!F1:N4,1,1)</f>

</xml_diff>

<commit_message>
Fixing up Pooled methods
These methods now work for the updated result structures for SFN. Will now be redoing some of the plots on a bigger computer screen
</commit_message>
<xml_diff>
--- a/Results/Pooled Analyses/SfN2017/SfN2017Stat.xlsx
+++ b/Results/Pooled Analyses/SfN2017/SfN2017Stat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\MATLAB\Dissociating-Role-of-Feedback-in-Voice-Motor-Control\Results\Pooled Analyses\SfN2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djsmith\Documents\MATLAB\Dissociating-Role-of-Feedback-in-Voice-Motor-Control\Results\Pooled Analyses\SfN2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,118 +399,118 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>-48.242649518285319</v>
+        <v>-47.093411805028012</v>
       </c>
       <c r="B1">
-        <v>-46.815454639102917</v>
+        <v>-45.796570636779407</v>
       </c>
       <c r="C1">
-        <v>25.467418578267914</v>
+        <v>24.326001492432852</v>
       </c>
       <c r="D1">
-        <v>17.574269392807071</v>
+        <v>17.626031549730353</v>
       </c>
       <c r="E1">
-        <v>56.051484437544296</v>
+        <v>54.438998573787885</v>
       </c>
       <c r="F1">
-        <v>23.739806067855504</v>
+        <v>35.313186192113037</v>
       </c>
       <c r="G1">
-        <v>0.82077446204103555</v>
+        <v>0.81638124054605699</v>
       </c>
       <c r="H1">
-        <v>0.15002041082696027</v>
+        <v>0.20978629136840976</v>
       </c>
       <c r="I1">
-        <v>6.2873566091793481E-2</v>
+        <v>5.9078591904416292E-2</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-38.568789654826901</v>
+        <v>-38.265634945855453</v>
       </c>
       <c r="B2">
-        <v>-37.058758765709939</v>
+        <v>-37.635360113043362</v>
       </c>
       <c r="C2">
-        <v>39.652384484547859</v>
+        <v>38.712456830791211</v>
       </c>
       <c r="D2">
-        <v>22.233071697874685</v>
+        <v>23.016927870370008</v>
       </c>
       <c r="E2">
-        <v>112.06024561874294</v>
+        <v>105.62959350970402</v>
       </c>
       <c r="F2">
-        <v>44.848392915193649</v>
+        <v>35.787042247864107</v>
       </c>
       <c r="G2">
-        <v>0.77604792271659129</v>
+        <v>0.90498762369666896</v>
       </c>
       <c r="H2">
-        <v>2.338784622668174E-2</v>
+        <v>3.4968685182419405E-2</v>
       </c>
       <c r="I2">
-        <v>2.6059326658168607E-2</v>
+        <v>2.0731388653787819E-2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>-32.855435271891913</v>
+        <v>-31.571276733407295</v>
       </c>
       <c r="B3">
-        <v>-19.364946692964853</v>
+        <v>-15.939521141709742</v>
       </c>
       <c r="C3">
-        <v>24.886237802842782</v>
+        <v>24.791782046323892</v>
       </c>
       <c r="D3">
-        <v>26.523555712032437</v>
+        <v>22.854270814486988</v>
       </c>
       <c r="E3">
-        <v>73.584706403222611</v>
+        <v>81.88700034240496</v>
       </c>
       <c r="F3">
-        <v>96.300037659891615</v>
+        <v>102.24796447119215</v>
       </c>
       <c r="G3">
-        <v>1.7952714771327243E-2</v>
+        <v>2.5296428264772169E-3</v>
       </c>
       <c r="H3">
-        <v>0.84980120462270137</v>
+        <v>0.80934649864970498</v>
       </c>
       <c r="I3">
-        <v>0.54459077402851874</v>
+        <v>0.61691900283934253</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>-97.92097308662197</v>
+        <v>-93.827219101650854</v>
       </c>
       <c r="B4">
-        <v>-78.496639998254906</v>
+        <v>-75.259887621435894</v>
       </c>
       <c r="C4">
-        <v>23.813821668604032</v>
+        <v>20.524946103312175</v>
       </c>
       <c r="D4">
-        <v>24.106221427066124</v>
+        <v>24.524406722136476</v>
       </c>
       <c r="E4">
-        <v>23.508923601223366</v>
+        <v>22.656434572086848</v>
       </c>
       <c r="F4">
-        <v>32.330468954191872</v>
+        <v>34.629856974980676</v>
       </c>
       <c r="G4">
-        <v>6.403038201997592E-2</v>
+        <v>7.7412085834651881E-2</v>
       </c>
       <c r="H4">
-        <v>0.97731086153151481</v>
+        <v>0.6894181029641091</v>
       </c>
       <c r="I4">
-        <v>0.60931132471887395</v>
+        <v>0.40548889126828125</v>
       </c>
     </row>
   </sheetData>
@@ -585,27 +585,27 @@
       </c>
       <c r="B5" s="2">
         <f>INDEX(Sheet1!A1:I4,1,1)</f>
-        <v>-48.242649518285319</v>
+        <v>-47.093411805028012</v>
       </c>
       <c r="C5" s="2">
         <f>INDEX(Sheet1!B1:J4,1,1)</f>
-        <v>-46.815454639102917</v>
+        <v>-45.796570636779407</v>
       </c>
       <c r="D5" s="2">
         <f>INDEX(Sheet1!C1:K4,1,1)</f>
-        <v>25.467418578267914</v>
+        <v>24.326001492432852</v>
       </c>
       <c r="E5" s="2">
         <f>INDEX(Sheet1!D1:L4,1,1)</f>
-        <v>17.574269392807071</v>
+        <v>17.626031549730353</v>
       </c>
       <c r="F5" s="3">
         <f>INDEX(Sheet1!E1:M4,1,1)</f>
-        <v>56.051484437544296</v>
+        <v>54.438998573787885</v>
       </c>
       <c r="G5" s="3">
         <f>INDEX(Sheet1!F1:N4,1,1)</f>
-        <v>23.739806067855504</v>
+        <v>35.313186192113037</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -614,27 +614,27 @@
       </c>
       <c r="B6" s="2">
         <f>INDEX(Sheet1!A2:I5,1,1)</f>
-        <v>-38.568789654826901</v>
+        <v>-38.265634945855453</v>
       </c>
       <c r="C6" s="2">
         <f>INDEX(Sheet1!B2:J5,1,1)</f>
-        <v>-37.058758765709939</v>
+        <v>-37.635360113043362</v>
       </c>
       <c r="D6" s="2">
         <f>INDEX(Sheet1!C2:K5,1,1)</f>
-        <v>39.652384484547859</v>
+        <v>38.712456830791211</v>
       </c>
       <c r="E6" s="2">
         <f>INDEX(Sheet1!D2:L5,1,1)</f>
-        <v>22.233071697874685</v>
+        <v>23.016927870370008</v>
       </c>
       <c r="F6" s="3">
         <f>INDEX(Sheet1!E2:M5,1,1)</f>
-        <v>112.06024561874294</v>
+        <v>105.62959350970402</v>
       </c>
       <c r="G6" s="3">
         <f>INDEX(Sheet1!F2:N5,1,1)</f>
-        <v>44.848392915193649</v>
+        <v>35.787042247864107</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -643,27 +643,27 @@
       </c>
       <c r="B7" s="2">
         <f>INDEX(Sheet1!A3:I6,1,1)</f>
-        <v>-32.855435271891913</v>
+        <v>-31.571276733407295</v>
       </c>
       <c r="C7" s="2">
         <f>INDEX(Sheet1!B3:J6,1,1)</f>
-        <v>-19.364946692964853</v>
+        <v>-15.939521141709742</v>
       </c>
       <c r="D7" s="2">
         <f>INDEX(Sheet1!C3:K6,1,1)</f>
-        <v>24.886237802842782</v>
+        <v>24.791782046323892</v>
       </c>
       <c r="E7" s="2">
         <f>INDEX(Sheet1!D3:L6,1,1)</f>
-        <v>26.523555712032437</v>
+        <v>22.854270814486988</v>
       </c>
       <c r="F7" s="3">
         <f>INDEX(Sheet1!E3:M6,1,1)</f>
-        <v>73.584706403222611</v>
+        <v>81.88700034240496</v>
       </c>
       <c r="G7" s="3">
         <f>INDEX(Sheet1!F3:N6,1,1)</f>
-        <v>96.300037659891615</v>
+        <v>102.24796447119215</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -672,27 +672,27 @@
       </c>
       <c r="B8" s="2">
         <f>INDEX(Sheet1!A4:I7,1,1)</f>
-        <v>-97.92097308662197</v>
+        <v>-93.827219101650854</v>
       </c>
       <c r="C8" s="2">
         <f>INDEX(Sheet1!B4:J7,1,1)</f>
-        <v>-78.496639998254906</v>
+        <v>-75.259887621435894</v>
       </c>
       <c r="D8" s="2">
         <f>INDEX(Sheet1!C4:K7,1,1)</f>
-        <v>23.813821668604032</v>
+        <v>20.524946103312175</v>
       </c>
       <c r="E8" s="2">
         <f>INDEX(Sheet1!D4:L7,1,1)</f>
-        <v>24.106221427066124</v>
+        <v>24.524406722136476</v>
       </c>
       <c r="F8" s="3">
         <f>INDEX(Sheet1!E4:M7,1,1)</f>
-        <v>23.508923601223366</v>
+        <v>22.656434572086848</v>
       </c>
       <c r="G8" s="3">
         <f>INDEX(Sheet1!F4:N7,1,1)</f>
-        <v>32.330468954191872</v>
+        <v>34.629856974980676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>